<commit_message>
Updated report and benchmark
</commit_message>
<xml_diff>
--- a/benchmarking.xlsx
+++ b/benchmarking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Documents\GitHub\cs9417\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D31337-F41F-4B32-A11E-3D4E5E927246}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B300DC9A-EBB6-4167-BC75-181539E09170}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="1" xr2:uid="{EFD9CA6E-104E-4ED9-94EB-F6073527FC27}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="3" xr2:uid="{EFD9CA6E-104E-4ED9-94EB-F6073527FC27}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="4" r:id="rId1"/>
@@ -80,7 +80,7 @@
     <numFmt numFmtId="164" formatCode="0.00000000000000%"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +110,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -132,13 +138,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1608,7 +1615,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,8 +1692,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB6D85D-E31E-46C2-BB04-3D7E8AFEFB10}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,7 +2117,10 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="E6:G6"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,6 +2223,12 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
+      <c r="E6" s="6">
+        <v>192</v>
+      </c>
+      <c r="F6" s="6">
+        <v>6706</v>
+      </c>
       <c r="I6" t="s">
         <v>4</v>
       </c>
@@ -2226,7 +2245,7 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G7">
         <f>SUM(D4:F6)</f>
-        <v>2724</v>
+        <v>9622</v>
       </c>
       <c r="N7">
         <f>SUM(K4:M6)</f>
@@ -2236,15 +2255,15 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F9">
         <f>(E5+F6+D4+C3)/4+(D4+E5+C3)/2+SUM(C3:E5)/4</f>
-        <v>2063.25</v>
+        <v>3739.75</v>
       </c>
       <c r="G9">
         <f>G7/4+SUM(C3:F5)*3/4</f>
-        <v>2724</v>
+        <v>4448.5</v>
       </c>
       <c r="H9" s="1">
         <f>F9/G9</f>
-        <v>0.75743392070484583</v>
+        <v>0.84067663257277736</v>
       </c>
       <c r="M9">
         <f>(L5+M6+K4+J3)/4+(K4+L5+J3)/2+SUM(J3:L5)/4</f>
@@ -2611,8 +2630,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F904C3-3753-41C0-ABE8-80B27895448C}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2721,6 +2743,13 @@
       <c r="B5" t="s">
         <v>1</v>
       </c>
+      <c r="D5" s="6">
+        <v>101</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1699</v>
+      </c>
+      <c r="F5" s="6"/>
       <c r="I5" t="s">
         <v>1</v>
       </c>
@@ -2740,6 +2769,13 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6">
+        <v>192</v>
+      </c>
+      <c r="F6" s="6">
+        <v>6706</v>
       </c>
       <c r="I6" t="s">
         <v>4</v>
@@ -2760,7 +2796,7 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G7">
         <f>SUM(C3:F6)</f>
-        <v>924</v>
+        <v>9622</v>
       </c>
       <c r="N7">
         <f>SUM(J3:M6)</f>
@@ -2770,15 +2806,15 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F9">
         <f>(E5+F6+D4+C3)/4+(D4+E5+C3)/2+SUM(C3:E5)/4</f>
-        <v>799.5</v>
+        <v>4200.25</v>
       </c>
       <c r="G9">
         <f>G7/4+SUM(C3:F5)*3/4</f>
-        <v>924</v>
+        <v>4448.5</v>
       </c>
       <c r="H9" s="1">
         <f>F9/G9</f>
-        <v>0.86525974025974028</v>
+        <v>0.94419467236147014</v>
       </c>
       <c r="M9">
         <f>(L5+M6+K4+J3)/4+(K4+L5+J3)/2+SUM(J3:L5)/4</f>

</xml_diff>

<commit_message>
Updated benchmark and report
</commit_message>
<xml_diff>
--- a/benchmarking.xlsx
+++ b/benchmarking.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julian\Documents\GitHub\cs9417\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D31337-F41F-4B32-A11E-3D4E5E927246}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE3E808-8789-4EDE-A23E-46035AAF3334}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="1" xr2:uid="{EFD9CA6E-104E-4ED9-94EB-F6073527FC27}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="3" xr2:uid="{EFD9CA6E-104E-4ED9-94EB-F6073527FC27}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="4" r:id="rId1"/>
     <sheet name="word_overlap_all" sheetId="1" r:id="rId2"/>
     <sheet name="word_overlap_related" sheetId="2" r:id="rId3"/>
     <sheet name="word_overlap_biased" sheetId="3" r:id="rId4"/>
+    <sheet name="paraphrase_all" sheetId="5" r:id="rId5"/>
+    <sheet name="paraphrase_related" sheetId="6" r:id="rId6"/>
+    <sheet name="paraphrase_biased" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="16">
   <si>
     <t>goal\test</t>
   </si>
@@ -70,6 +73,12 @@
   </si>
   <si>
     <t>DIFF</t>
+  </si>
+  <si>
+    <t>WORD_OVERLAP</t>
+  </si>
+  <si>
+    <t>PARAPHRASE</t>
   </si>
 </sst>
 </file>
@@ -174,34 +183,27 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Comparison!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DIFF</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Word Overlap</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Comparison!$A$2:$A$4</c:f>
@@ -237,40 +239,18 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-56EB-488A-B60C-59B652F0A4C4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="10703072"/>
-        <c:axId val="6039808"/>
-      </c:barChart>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Comparison!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>OURS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Paraphrasing</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -286,18 +266,18 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Comparison!$C$2:$C$4</c:f>
+              <c:f>Comparison!$F$2:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.92357043235704328</c:v>
+                  <c:v>4.3171333547902591E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77487394056431713</c:v>
+                  <c:v>5.089582662804415E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76901619997854309</c:v>
+                  <c:v>3.3515717197725614E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -317,10 +297,9 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1524320704"/>
-        <c:axId val="11545888"/>
+        <c:axId val="10703072"/>
+        <c:axId val="6039808"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="10703072"/>
@@ -470,8 +449,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-AU"/>
-                  <a:t>Relative Improvement</a:t>
+                  <a:t>Relative Improvement on Competition</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> Set vs. Baseline</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -539,126 +523,6 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:valAx>
-        <c:axId val="11545888"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0.60000000000000009"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU"/>
-                  <a:t>Our</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t> Score %</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-AU"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1524320704"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="1524320704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="11545888"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -667,6 +531,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1605,26 +1500,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1253E610-1417-4D91-A0E3-CE38B43A3CD3}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1637,11 +1544,19 @@
         <v>0.92357043235704328</v>
       </c>
       <c r="D2" s="5">
-        <f>C2-B2</f>
+        <f>C2-$B2</f>
         <v>3.4781675785859889E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3">
+        <f>paraphrase_all!O9</f>
+        <v>0.93196009011908598</v>
+      </c>
+      <c r="F2" s="5">
+        <f>E2-$B2</f>
+        <v>4.3171333547902591E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1654,11 +1569,19 @@
         <v>0.77487394056431713</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D4" si="0">C3-B3</f>
+        <f t="shared" ref="D3:F4" si="0">C3-$B3</f>
         <v>1.9718914279583721E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3">
+        <f>paraphrase_related!O9</f>
+        <v>0.80605085291277756</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="shared" si="0"/>
+        <v>5.089582662804415E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1673,6 +1596,14 @@
       <c r="D4" s="5">
         <f t="shared" si="0"/>
         <v>1.7015341701534181E-2</v>
+      </c>
+      <c r="E4" s="3">
+        <f>paraphrase_biased!O9</f>
+        <v>0.78551657547473452</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
+        <v>3.3515717197725614E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1685,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB6D85D-E31E-46C2-BB04-3D7E8AFEFB10}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,7 +2038,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="E6:G6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,6 +2141,12 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
+      <c r="E6">
+        <v>192</v>
+      </c>
+      <c r="F6">
+        <v>6706</v>
+      </c>
       <c r="I6" t="s">
         <v>4</v>
       </c>
@@ -2226,7 +2163,7 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G7">
         <f>SUM(D4:F6)</f>
-        <v>2724</v>
+        <v>9622</v>
       </c>
       <c r="N7">
         <f>SUM(K4:M6)</f>
@@ -2236,15 +2173,15 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F9">
         <f>(E5+F6+D4+C3)/4+(D4+E5+C3)/2+SUM(C3:E5)/4</f>
-        <v>2063.25</v>
+        <v>3739.75</v>
       </c>
       <c r="G9">
         <f>G7/4+SUM(C3:F5)*3/4</f>
-        <v>2724</v>
+        <v>4448.5</v>
       </c>
       <c r="H9" s="1">
         <f>F9/G9</f>
-        <v>0.75743392070484583</v>
+        <v>0.84067663257277736</v>
       </c>
       <c r="M9">
         <f>(L5+M6+K4+J3)/4+(K4+L5+J3)/2+SUM(J3:L5)/4</f>
@@ -2609,6 +2546,1538 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F904C3-3753-41C0-ABE8-80B27895448C}">
+  <dimension ref="A1:O26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>753</v>
+      </c>
+      <c r="D3" s="4">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4">
+        <v>247</v>
+      </c>
+      <c r="K3" s="4">
+        <v>17</v>
+      </c>
+      <c r="L3">
+        <v>1456</v>
+      </c>
+      <c r="M3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>157</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="4">
+        <v>74</v>
+      </c>
+      <c r="K4" s="4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>468</v>
+      </c>
+      <c r="M4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>101</v>
+      </c>
+      <c r="E5">
+        <v>1699</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>358</v>
+      </c>
+      <c r="K5">
+        <v>28</v>
+      </c>
+      <c r="L5">
+        <v>3666</v>
+      </c>
+      <c r="M5">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>192</v>
+      </c>
+      <c r="F6">
+        <v>6706</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>23</v>
+      </c>
+      <c r="K6">
+        <v>7</v>
+      </c>
+      <c r="L6">
+        <v>564</v>
+      </c>
+      <c r="M6">
+        <v>17755</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>SUM(C3:F6)</f>
+        <v>9622</v>
+      </c>
+      <c r="N7">
+        <f>SUM(J3:M6)</f>
+        <v>25413</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f>(E5+F6+D4+C3)/4+(D4+E5+C3)/2+SUM(C3:E5)/4</f>
+        <v>4200.25</v>
+      </c>
+      <c r="G9">
+        <f>G7/4+SUM(C3:F5)*3/4</f>
+        <v>4448.5</v>
+      </c>
+      <c r="H9" s="1">
+        <f>F9/G9</f>
+        <v>0.94419467236147014</v>
+      </c>
+      <c r="M9">
+        <f>(L5+M6+K4+J3)/4+(K4+L5+J3)/2+SUM(J3:L5)/4</f>
+        <v>8960</v>
+      </c>
+      <c r="N9">
+        <f>N7/4+SUM(J3:M5)*3/4</f>
+        <v>11651.25</v>
+      </c>
+      <c r="O9" s="1">
+        <f>M9/N9</f>
+        <v>0.76901619997854309</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>118</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>556</v>
+      </c>
+      <c r="F12">
+        <v>85</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>173</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>1435</v>
+      </c>
+      <c r="M12">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>130</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>39</v>
+      </c>
+      <c r="K13">
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <v>413</v>
+      </c>
+      <c r="M13">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>58</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>1527</v>
+      </c>
+      <c r="F14">
+        <v>210</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>221</v>
+      </c>
+      <c r="K14">
+        <v>7</v>
+      </c>
+      <c r="L14">
+        <v>3556</v>
+      </c>
+      <c r="M14">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>98</v>
+      </c>
+      <c r="F15">
+        <v>6794</v>
+      </c>
+      <c r="I15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <v>358</v>
+      </c>
+      <c r="M15">
+        <v>17978</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f>SUM(C12:F15)</f>
+        <v>9622</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="N16">
+        <f>SUM(J12:M15)</f>
+        <v>25413</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f>SUM(C12:E14)</f>
+        <v>2414</v>
+      </c>
+      <c r="L17">
+        <f>SUM(J12:L14)</f>
+        <v>5861</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" t="s">
+        <v>3</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:F20" si="0">C12</f>
+        <v>118</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>556</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="I20" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>173</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20">
+        <v>1435</v>
+      </c>
+      <c r="M20">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:F21" si="1">C13</f>
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <v>39</v>
+      </c>
+      <c r="K21">
+        <v>7</v>
+      </c>
+      <c r="L21">
+        <v>413</v>
+      </c>
+      <c r="M21">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:F22" si="2">C14</f>
+        <v>58</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>1527</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>210</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>221</v>
+      </c>
+      <c r="K22">
+        <v>7</v>
+      </c>
+      <c r="L22">
+        <v>3556</v>
+      </c>
+      <c r="M22">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:E23" si="3">C15</f>
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="F23">
+        <f>F15</f>
+        <v>6794</v>
+      </c>
+      <c r="I23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>10</v>
+      </c>
+      <c r="K23">
+        <v>3</v>
+      </c>
+      <c r="L23">
+        <v>358</v>
+      </c>
+      <c r="M23">
+        <v>17978</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f>SUM(C20:F23)</f>
+        <v>9622</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="N24">
+        <f>SUM(J20:M23)</f>
+        <v>25413</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f>(E22+F23+D21+C20)/4+(D21+E22+C20)/2+SUM(C20:E22)/4</f>
+        <v>3538</v>
+      </c>
+      <c r="G26">
+        <f>G24/4+SUM(C20:F22)*3/4</f>
+        <v>4448.5</v>
+      </c>
+      <c r="H26" s="1">
+        <f>F26/G26</f>
+        <v>0.7953242666067214</v>
+      </c>
+      <c r="M26">
+        <f>(L22+M23+K21+J20)/4+(K21+L22+J20)/2+SUM(J20:L22)/4</f>
+        <v>8761.75</v>
+      </c>
+      <c r="N26">
+        <f>N24/4+SUM(J20:M22)*3/4</f>
+        <v>11651.25</v>
+      </c>
+      <c r="O26" s="1">
+        <f>M26/N26</f>
+        <v>0.75200085827700891</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE46BCF1-F0AE-4D2D-A293-89960E44BE03}">
+  <dimension ref="A1:O26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <f>695+153+1630</f>
+        <v>2478</v>
+      </c>
+      <c r="F5" s="4">
+        <f>67+9+170</f>
+        <v>246</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
+        <f>1745+572+4095</f>
+        <v>6412</v>
+      </c>
+      <c r="M5" s="4">
+        <f>158+125+369</f>
+        <v>652</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4">
+        <v>173</v>
+      </c>
+      <c r="F6" s="4">
+        <v>6725</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="4">
+        <v>563</v>
+      </c>
+      <c r="M6" s="4">
+        <v>17786</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>SUM(E5:F6)</f>
+        <v>9622</v>
+      </c>
+      <c r="N7">
+        <f>SUM(L5:M6)</f>
+        <v>25413</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f>(E5+F6+D4+C3)/4+(D4+E5+C3)/2+SUM(C3:E5)/4</f>
+        <v>4159.25</v>
+      </c>
+      <c r="G9">
+        <f>G7/4+SUM(C3:F5)*3/4</f>
+        <v>4448.5</v>
+      </c>
+      <c r="H9" s="1">
+        <f>F9/G9</f>
+        <v>0.93497808249971903</v>
+      </c>
+      <c r="M9">
+        <f>(L5+M6+K4+J3)/4+(K4+L5+J3)/2+SUM(J3:L5)/4</f>
+        <v>10858.5</v>
+      </c>
+      <c r="N9">
+        <f>N7/4+SUM(J3:M5)*3/4</f>
+        <v>11651.25</v>
+      </c>
+      <c r="O9" s="1">
+        <f>M9/N9</f>
+        <v>0.93196009011908598</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>118</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>556</v>
+      </c>
+      <c r="F12">
+        <v>85</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>173</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>1435</v>
+      </c>
+      <c r="M12">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>130</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>39</v>
+      </c>
+      <c r="K13">
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <v>413</v>
+      </c>
+      <c r="M13">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>58</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>1527</v>
+      </c>
+      <c r="F14">
+        <v>210</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>221</v>
+      </c>
+      <c r="K14">
+        <v>7</v>
+      </c>
+      <c r="L14">
+        <v>3556</v>
+      </c>
+      <c r="M14">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>98</v>
+      </c>
+      <c r="F15">
+        <v>6794</v>
+      </c>
+      <c r="I15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <v>358</v>
+      </c>
+      <c r="M15">
+        <v>17978</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f>SUM(C12:F15)</f>
+        <v>9622</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="N16">
+        <f>SUM(J12:M15)</f>
+        <v>25413</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f>SUM(C12:E14)</f>
+        <v>2414</v>
+      </c>
+      <c r="L17">
+        <f>SUM(J12:L14)</f>
+        <v>5861</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <f>SUM(C12:E14)</f>
+        <v>2414</v>
+      </c>
+      <c r="F22">
+        <f>SUM(F12:F14)</f>
+        <v>310</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <f>SUM(J12:L14)</f>
+        <v>5861</v>
+      </c>
+      <c r="M22">
+        <f>SUM(M12:M14)</f>
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <f>SUM(C15:E15)</f>
+        <v>104</v>
+      </c>
+      <c r="F23">
+        <f>F15</f>
+        <v>6794</v>
+      </c>
+      <c r="I23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <f>SUM(J15:L15)</f>
+        <v>371</v>
+      </c>
+      <c r="M23">
+        <f>M15</f>
+        <v>17978</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f>SUM(E22:F23)</f>
+        <v>9622</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="N24">
+        <f>SUM(L22:M23)</f>
+        <v>25413</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f>(E22+F23+D21+C20)/4+(D21+E22+C20)/2+SUM(C20:E22)/4</f>
+        <v>4112.5</v>
+      </c>
+      <c r="G26">
+        <f>G24/4+SUM(C20:F22)*3/4</f>
+        <v>4448.5</v>
+      </c>
+      <c r="H26" s="1">
+        <f>F26/G26</f>
+        <v>0.9244689221085759</v>
+      </c>
+      <c r="M26">
+        <f>(L22+M23+K21+J20)/4+(K21+L22+J20)/2+SUM(J20:L22)/4</f>
+        <v>10355.5</v>
+      </c>
+      <c r="N26">
+        <f>N24/4+SUM(J20:M22)*3/4</f>
+        <v>11651.25</v>
+      </c>
+      <c r="O26" s="1">
+        <f>M26/N26</f>
+        <v>0.88878875657118339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714E8E23-A025-4956-BCBD-8EA7279EF20A}">
+  <dimension ref="A1:O26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <f>412+102</f>
+        <v>514</v>
+      </c>
+      <c r="E4" s="4">
+        <f>350+60</f>
+        <v>410</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="4">
+        <f>997+310</f>
+        <v>1307</v>
+      </c>
+      <c r="L4" s="4">
+        <f>748+262</f>
+        <v>1010</v>
+      </c>
+      <c r="M4">
+        <f>158+125</f>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>194</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1606</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>946</v>
+      </c>
+      <c r="L5" s="4">
+        <v>3149</v>
+      </c>
+      <c r="M5">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>173</v>
+      </c>
+      <c r="F6">
+        <v>6725</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>163</v>
+      </c>
+      <c r="L6">
+        <v>400</v>
+      </c>
+      <c r="M6">
+        <v>17786</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>SUM(D4:F6)</f>
+        <v>9622</v>
+      </c>
+      <c r="N7">
+        <f>SUM(K4:M6)</f>
+        <v>25413</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f>(E5+F6+D4+C3)/4+(D4+E5+C3)/2+SUM(C3:E5)/4</f>
+        <v>3952.25</v>
+      </c>
+      <c r="G9">
+        <f>G7/4+SUM(C3:F5)*3/4</f>
+        <v>4448.5</v>
+      </c>
+      <c r="H9" s="1">
+        <f>F9/G9</f>
+        <v>0.88844554344160953</v>
+      </c>
+      <c r="M9">
+        <f>(L5+M6+K4+J3)/4+(K4+L5+J3)/2+SUM(J3:L5)/4</f>
+        <v>9391.5</v>
+      </c>
+      <c r="N9">
+        <f>N7/4+SUM(J3:M5)*3/4</f>
+        <v>11651.25</v>
+      </c>
+      <c r="O9" s="1">
+        <f>M9/N9</f>
+        <v>0.80605085291277756</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>118</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>556</v>
+      </c>
+      <c r="F12">
+        <v>85</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>173</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>1435</v>
+      </c>
+      <c r="M12">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>130</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>39</v>
+      </c>
+      <c r="K13">
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <v>413</v>
+      </c>
+      <c r="M13">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>58</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>1527</v>
+      </c>
+      <c r="F14">
+        <v>210</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>221</v>
+      </c>
+      <c r="K14">
+        <v>7</v>
+      </c>
+      <c r="L14">
+        <v>3556</v>
+      </c>
+      <c r="M14">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>98</v>
+      </c>
+      <c r="F15">
+        <v>6794</v>
+      </c>
+      <c r="I15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <v>358</v>
+      </c>
+      <c r="M15">
+        <v>17978</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f>SUM(C12:F15)</f>
+        <v>9622</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="N16">
+        <f>SUM(J12:M15)</f>
+        <v>25413</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f>SUM(C12:E14)</f>
+        <v>2414</v>
+      </c>
+      <c r="L17">
+        <f>SUM(J12:L14)</f>
+        <v>5861</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <f>SUM(C12:D13)</f>
+        <v>138</v>
+      </c>
+      <c r="E21">
+        <f>SUM(E12:E13)</f>
+        <v>686</v>
+      </c>
+      <c r="F21">
+        <f>SUM(F12:F13)</f>
+        <v>100</v>
+      </c>
+      <c r="I21" t="s">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <f>SUM(J12:K13)</f>
+        <v>229</v>
+      </c>
+      <c r="L21">
+        <f>SUM(L12:L13)</f>
+        <v>1848</v>
+      </c>
+      <c r="M21">
+        <f>SUM(M12:M13)</f>
+        <v>523</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f>SUM(C14:D14)</f>
+        <v>63</v>
+      </c>
+      <c r="E22">
+        <f>E14</f>
+        <v>1527</v>
+      </c>
+      <c r="F22">
+        <f>F14</f>
+        <v>210</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <f>SUM(J14:K14)</f>
+        <v>228</v>
+      </c>
+      <c r="L22">
+        <f>L14</f>
+        <v>3556</v>
+      </c>
+      <c r="M22">
+        <f>M14</f>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <f>SUM(C15:D15)</f>
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <f>E15</f>
+        <v>98</v>
+      </c>
+      <c r="F23">
+        <f>F15</f>
+        <v>6794</v>
+      </c>
+      <c r="I23" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23">
+        <f>SUM(J15:K15)</f>
+        <v>13</v>
+      </c>
+      <c r="L23">
+        <f>L15</f>
+        <v>358</v>
+      </c>
+      <c r="M23">
+        <f>M15</f>
+        <v>17978</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f>SUM(D21:F23)</f>
+        <v>9622</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="N24">
+        <f>SUM(K21:M23)</f>
+        <v>25413</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f>(E22+F23+D21+C20)/4+(D21+E22+C20)/2+SUM(C20:E22)/4</f>
+        <v>3550.75</v>
+      </c>
+      <c r="G26">
+        <f>G24/4+SUM(C20:F22)*3/4</f>
+        <v>4448.5</v>
+      </c>
+      <c r="H26" s="1">
+        <f>F26/G26</f>
+        <v>0.79819040125885132</v>
+      </c>
+      <c r="M26">
+        <f>(L22+M23+K21+J20)/4+(K21+L22+J20)/2+SUM(J20:L22)/4</f>
+        <v>8798.5</v>
+      </c>
+      <c r="N26">
+        <f>N24/4+SUM(J20:M22)*3/4</f>
+        <v>11651.25</v>
+      </c>
+      <c r="O26" s="1">
+        <f>M26/N26</f>
+        <v>0.75515502628473341</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C3D47F-1560-4850-83E5-477801F6ABCE}">
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2670,25 +4139,25 @@
         <v>2</v>
       </c>
       <c r="C3" s="4">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="D3" s="4">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="4">
-        <v>247</v>
+        <v>971</v>
       </c>
       <c r="K3" s="4">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="L3">
-        <v>1456</v>
+        <v>748</v>
       </c>
       <c r="M3">
-        <v>183</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2696,71 +4165,83 @@
         <v>3</v>
       </c>
       <c r="C4" s="4">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D4" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="4">
-        <v>74</v>
+        <v>293</v>
       </c>
       <c r="K4" s="4">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="L4">
-        <v>468</v>
+        <v>262</v>
       </c>
       <c r="M4">
-        <v>147</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
+      <c r="D5">
+        <v>194</v>
+      </c>
+      <c r="E5">
+        <v>1606</v>
+      </c>
       <c r="I5" t="s">
         <v>1</v>
       </c>
       <c r="J5">
-        <v>358</v>
+        <v>924</v>
       </c>
       <c r="K5">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L5">
-        <v>3666</v>
+        <v>3149</v>
       </c>
       <c r="M5">
-        <v>412</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
+      <c r="E6">
+        <v>173</v>
+      </c>
+      <c r="F6">
+        <v>6725</v>
+      </c>
       <c r="I6" t="s">
         <v>4</v>
       </c>
       <c r="J6">
-        <v>23</v>
+        <v>157</v>
       </c>
       <c r="K6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L6">
-        <v>564</v>
+        <v>400</v>
       </c>
       <c r="M6">
-        <v>17755</v>
+        <v>17786</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G7">
         <f>SUM(C3:F6)</f>
-        <v>924</v>
+        <v>9622</v>
       </c>
       <c r="N7">
         <f>SUM(J3:M6)</f>
@@ -2770,19 +4251,19 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F9">
         <f>(E5+F6+D4+C3)/4+(D4+E5+C3)/2+SUM(C3:E5)/4</f>
-        <v>799.5</v>
+        <v>4132.25</v>
       </c>
       <c r="G9">
         <f>G7/4+SUM(C3:F5)*3/4</f>
-        <v>924</v>
+        <v>4448.5</v>
       </c>
       <c r="H9" s="1">
         <f>F9/G9</f>
-        <v>0.86525974025974028</v>
+        <v>0.92890862088344384</v>
       </c>
       <c r="M9">
         <f>(L5+M6+K4+J3)/4+(K4+L5+J3)/2+SUM(J3:L5)/4</f>
-        <v>8960</v>
+        <v>9152.25</v>
       </c>
       <c r="N9">
         <f>N7/4+SUM(J3:M5)*3/4</f>
@@ -2790,7 +4271,7 @@
       </c>
       <c r="O9" s="1">
         <f>M9/N9</f>
-        <v>0.76901619997854309</v>
+        <v>0.78551657547473452</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -3014,7 +4495,7 @@
         <v>2</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:F20" si="0">C12</f>
+        <f t="shared" ref="C20:F23" si="0">C12</f>
         <v>118</v>
       </c>
       <c r="D20">
@@ -3050,19 +4531,19 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:F21" si="1">C13</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="I21" t="s">
@@ -3086,19 +4567,19 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:F22" si="2">C14</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="D22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1527</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="I22" t="s">
@@ -3122,15 +4603,15 @@
         <v>4</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:E23" si="3">C15</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>98</v>
       </c>
       <c r="F23">

</xml_diff>